<commit_message>
Added analysis for MaxQuant and Proteome Discoverer
Changed R script to also allow for analysis of MaxQuant and Proteome Discoverer output data, in addition to DiaNN output data. Analysis_parameters file was altered accordingly
</commit_message>
<xml_diff>
--- a/Analysis_parameters.xlsx
+++ b/Analysis_parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dick\Post-doc\Analysis scripts\DiaNN basic post-processing\Testing folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dick\Post-doc\Analysis scripts\MS basic post-processing\All_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F460C181-4315-4805-9401-6C0EC9113E78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8975E2A-745F-4582-B275-B3EB2AEA603F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5AB9C566-9F07-4C33-B851-369A57D17F28}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{5AB9C566-9F07-4C33-B851-369A57D17F28}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>filtering_type</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>WT</t>
+  </si>
+  <si>
+    <t>Analysis method</t>
+  </si>
+  <si>
+    <t>Proteome Discoverer</t>
   </si>
 </sst>
 </file>
@@ -408,60 +414,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79C10FB2-336F-4851-BC33-70582F98C0E5}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="G18:H18"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="5">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" prompt="The amount of experimental variables. This can be either 2 (Condition A, Replicates) or 3 (Condition B, Condition A, Replicates). These variables should be present in the .raw file names._x000a_Condition A example: Cell lines_x000a_Condition B example: WT/KO" sqref="A2" xr:uid="{5282C8AD-1561-44E0-A80B-84CE01E96738}">
+  <dataValidations count="6">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" prompt="The amount of experimental variables. This can be either 2 (Condition A, Replicates) or 3 (Condition B, Condition A, Replicates). These variables should be present in the .raw file names._x000a_Condition A example: Cell lines_x000a_Condition B example: WT/KO" sqref="B2" xr:uid="{5282C8AD-1561-44E0-A80B-84CE01E96738}">
       <formula1>"2, 3"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" prompt="The type of comparison that will be tested. This can be all possible pairwise comparisons (&quot;all&quot;), limited to the comparisons versus the control (&quot;control&quot;), or manually defined contrasts (&quot;manual&quot;)." sqref="D2" xr:uid="{C495E0AF-0FD2-459F-A3CE-5F10744ED4BB}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" prompt="The type of comparison that will be tested. This can be all possible pairwise comparisons (&quot;all&quot;), limited to the comparisons versus the control (&quot;control&quot;), or manually defined contrasts (&quot;manual&quot;)." sqref="E2" xr:uid="{C495E0AF-0FD2-459F-A3CE-5F10744ED4BB}">
       <formula1>"control, all, manual"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Control sample" prompt="In case you choose &quot;control&quot; as your comparison, add the name of the control sample, e.g. DMSO, IgG, untreated, KO" sqref="E2" xr:uid="{FBBE24AB-7FB5-4AFC-8068-8D0236696CFE}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Mass spectrometer" prompt="This should be the same as in the names of the .raw files" sqref="C2" xr:uid="{68E78BE4-A7EB-420A-9A7C-D7D367FCB586}"/>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" prompt="This indicates the type of filtering_x000a__x000a_- complete: valid values in all samples_x000a_- condition: valid values in all samples of at least one group/condition" sqref="B2" xr:uid="{9FC734E1-D13B-4158-8BC3-0C7F48EE5CBD}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Control sample" prompt="In case you choose &quot;control&quot; as your comparison, add the name of the control sample, e.g. DMSO, IgG, untreated, KO" sqref="F2" xr:uid="{FBBE24AB-7FB5-4AFC-8068-8D0236696CFE}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Mass spectrometer" prompt="This should be the same as in the names of the .raw files" sqref="D2" xr:uid="{68E78BE4-A7EB-420A-9A7C-D7D367FCB586}"/>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" prompt="This indicates the type of filtering_x000a__x000a_- complete: valid values in all samples_x000a_- condition: valid values in all samples of at least one group/condition" sqref="C2" xr:uid="{9FC734E1-D13B-4158-8BC3-0C7F48EE5CBD}">
       <formula1>"complete, condition"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{01EF4A6D-0D3B-42B5-ADF2-F19004687B57}">
+      <formula1>"DiaNN, MaxQuant, Proteome Discoverer"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New features added and improved volcano plots
New features:

- Added parameter to filter based on the number of unique peptides
- Added BH correction to p-values
- Results are exported per contrast (2 conditions) and per contrast and condition B as a whole (3 conditions)
- Volcano plots are now made for each contrast seperately using ggplot2 and will have select proteins highlighted

Select which proteins are highlighted:
- Supply a list of proteins
- Based on criteria for significance (p-value and log2 FC)
- TopN most differential proteins that are below a set p-value
</commit_message>
<xml_diff>
--- a/Analysis_parameters.xlsx
+++ b/Analysis_parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dick\Post-doc\Analysis scripts\MS basic post-processing\All_tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dick\Post-doc\Analysis scripts\MS basic post-processing\Testing folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8975E2A-745F-4582-B275-B3EB2AEA603F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EAB6B95-8B56-44F0-B7C2-1B25636DB9AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{5AB9C566-9F07-4C33-B851-369A57D17F28}"/>
+    <workbookView xWindow="28680" yWindow="-1125" windowWidth="29040" windowHeight="17640" xr2:uid="{5AB9C566-9F07-4C33-B851-369A57D17F28}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>filtering_type</t>
   </si>
@@ -62,7 +62,31 @@
     <t>Analysis method</t>
   </si>
   <si>
-    <t>Proteome Discoverer</t>
+    <t>unique_peptides</t>
+  </si>
+  <si>
+    <t>proteins_to_highlight</t>
+  </si>
+  <si>
+    <t>volcano</t>
+  </si>
+  <si>
+    <t>p_value</t>
+  </si>
+  <si>
+    <t>log2_FC</t>
+  </si>
+  <si>
+    <t>TopN</t>
+  </si>
+  <si>
+    <t>specify significance</t>
+  </si>
+  <si>
+    <t>MaxQuant</t>
+  </si>
+  <si>
+    <t>EZH2;MBD3</t>
   </si>
 </sst>
 </file>
@@ -414,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79C10FB2-336F-4851-BC33-70582F98C0E5}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,7 +454,7 @@
     <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -449,10 +473,28 @@
       <c r="F1" t="s">
         <v>3</v>
       </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -469,23 +511,47 @@
       <c r="F2" t="s">
         <v>7</v>
       </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2">
+        <v>0.05</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="6">
+  <dataConsolidate/>
+  <dataValidations count="9">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" prompt="The amount of experimental variables. This can be either 2 (Condition A, Replicates) or 3 (Condition B, Condition A, Replicates). These variables should be present in the .raw file names._x000a_Condition A example: Cell lines_x000a_Condition B example: WT/KO" sqref="B2" xr:uid="{5282C8AD-1561-44E0-A80B-84CE01E96738}">
       <formula1>"2, 3"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" prompt="The type of comparison that will be tested. This can be all possible pairwise comparisons (&quot;all&quot;), limited to the comparisons versus the control (&quot;control&quot;), or manually defined contrasts (&quot;manual&quot;)." sqref="E2" xr:uid="{C495E0AF-0FD2-459F-A3CE-5F10744ED4BB}">
-      <formula1>"control, all, manual"</formula1>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" prompt="The type of comparison that will be tested. This can be all possible pairwise comparisons (&quot;all&quot;) or limited to the comparisons versus the control (&quot;control&quot;)." sqref="E2" xr:uid="{C495E0AF-0FD2-459F-A3CE-5F10744ED4BB}">
+      <formula1>"control, all"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Control sample" prompt="In case you choose &quot;control&quot; as your comparison, add the name of the control sample, e.g. DMSO, IgG, untreated, KO" sqref="F2" xr:uid="{FBBE24AB-7FB5-4AFC-8068-8D0236696CFE}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Mass spectrometer" prompt="This should be the same as in the names of the .raw files" sqref="D2" xr:uid="{68E78BE4-A7EB-420A-9A7C-D7D367FCB586}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Mass spectrometer" prompt="This should be present in the names of the .raw files. Required when selecting DiaNN as analysis method" sqref="D2" xr:uid="{68E78BE4-A7EB-420A-9A7C-D7D367FCB586}"/>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" prompt="This indicates the type of filtering_x000a__x000a_- complete: valid values in all samples_x000a_- condition: valid values in all samples of at least one group/condition" sqref="C2" xr:uid="{9FC734E1-D13B-4158-8BC3-0C7F48EE5CBD}">
       <formula1>"complete, condition"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{01EF4A6D-0D3B-42B5-ADF2-F19004687B57}">
       <formula1>"DiaNN, MaxQuant, Proteome Discoverer"</formula1>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The minimum amount of unique peptides a protein should be quantified with" sqref="G2" xr:uid="{A31E311C-361E-4F9F-B8B6-BC4E0E89553B}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Specifiy which proteins to highlight in the volcano plot._x000a_- list of supplied protein names or Uniprot IDs_x000a_- all proteins above a supplied p-value and fold change cutoff_x000a_- the top N most differential proteins with a p-value &lt; 0.05" sqref="H2" xr:uid="{A788C50D-30A4-4BCA-985C-C9490DA02A01}">
+      <formula1>"protein list, specify significance, TopN"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="List of proteins, separated by a semiolon (;)" sqref="I2" xr:uid="{E5F7B0FE-6278-49BC-987F-F5F080EF479D}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
v0.1.1 - Added option for complete export
New features:

- changed Analysis parameters to analysis_parameters for uniformity
- added filtering option for cRAP proteins present in ProteinGroup column for DiaNN analyses
- automatically install and load missing packages
- add option for export LFQ values raw, normalized and imputated values, together with all other dep object columns as 'complete_output'
</commit_message>
<xml_diff>
--- a/Analysis_parameters.xlsx
+++ b/Analysis_parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dick\Post-doc\Github\MS-basic-post-processing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dick\Post-doc\Analysis scripts\MS basic post-processing\All_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488E2254-0F9A-4FB8-AF4A-1A7812E88F88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2863AE5-E2AD-446B-935B-7AD5CE3666AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37080" yWindow="1305" windowWidth="21600" windowHeight="12735" xr2:uid="{5AB9C566-9F07-4C33-B851-369A57D17F28}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{5AB9C566-9F07-4C33-B851-369A57D17F28}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>filtering_type</t>
   </si>
@@ -59,9 +59,6 @@
     <t>WT</t>
   </si>
   <si>
-    <t>Analysis method</t>
-  </si>
-  <si>
     <t>unique_peptides</t>
   </si>
   <si>
@@ -83,10 +80,16 @@
     <t>specify significance</t>
   </si>
   <si>
-    <t>MaxQuant</t>
-  </si>
-  <si>
     <t>EZH2;MBD3</t>
+  </si>
+  <si>
+    <t>analysis_method</t>
+  </si>
+  <si>
+    <t>complete_output</t>
+  </si>
+  <si>
+    <t>DiaNN</t>
   </si>
 </sst>
 </file>
@@ -438,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79C10FB2-336F-4851-BC33-70582F98C0E5}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,9 +457,9 @@
     <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -474,27 +477,30 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>13</v>
       </c>
-      <c r="L1" t="s">
-        <v>14</v>
+      <c r="M1" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -515,10 +521,10 @@
         <v>2</v>
       </c>
       <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
         <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
       </c>
       <c r="J2">
         <v>0.05</v>
@@ -528,11 +534,14 @@
       </c>
       <c r="L2">
         <v>50</v>
+      </c>
+      <c r="M2" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <dataValidations count="9">
+  <dataValidations count="10">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" prompt="The amount of experimental variables. This can be either 2 (Condition A, Replicates) or 3 (Condition B, Condition A, Replicates). These variables should be present in the .raw file names._x000a_Condition A example: Cell lines_x000a_Condition B example: WT/KO" sqref="B2" xr:uid="{5282C8AD-1561-44E0-A80B-84CE01E96738}">
       <formula1>"2, 3"</formula1>
     </dataValidation>
@@ -552,6 +561,9 @@
       <formula1>"protein list, specify significance, TopN"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="List of proteins, separated by a semiolon (;)" sqref="I2" xr:uid="{E5F7B0FE-6278-49BC-987F-F5F080EF479D}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2" xr:uid="{BFA4E188-76D8-454E-913F-287D42E85D9F}">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update MS basic post-processing.R
- added option for highlighting imputed values (major)
- added option for manual contrasts (major)
- changed regex to separate on last underscore for experimental design (minor)
- changed max.overlaps = Inf for plotting (minor)
- Only export specific plots for imputed/non-imputed values (minor)
</commit_message>
<xml_diff>
--- a/Analysis_parameters.xlsx
+++ b/Analysis_parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dick\Post-doc\Analysis scripts\MS basic post-processing\All_tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dick\Post-doc\Analysis scripts\MS-basic-post-processing\All_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2863AE5-E2AD-446B-935B-7AD5CE3666AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA64554-29DE-4F95-9440-8AEB0FBF3C32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{5AB9C566-9F07-4C33-B851-369A57D17F28}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5AB9C566-9F07-4C33-B851-369A57D17F28}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>filtering_type</t>
   </si>
@@ -77,9 +77,6 @@
     <t>TopN</t>
   </si>
   <si>
-    <t>specify significance</t>
-  </si>
-  <si>
     <t>EZH2;MBD3</t>
   </si>
   <si>
@@ -90,6 +87,18 @@
   </si>
   <si>
     <t>DiaNN</t>
+  </si>
+  <si>
+    <t>highlight_imputed</t>
+  </si>
+  <si>
+    <t>contrasts</t>
+  </si>
+  <si>
+    <t>manual</t>
+  </si>
+  <si>
+    <t>MBD3GFP_vs_WT</t>
   </si>
 </sst>
 </file>
@@ -441,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79C10FB2-336F-4851-BC33-70582F98C0E5}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,12 +463,13 @@
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -474,33 +484,39 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>18</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -512,43 +528,46 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>2</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2">
+      <c r="K2">
         <v>0.05</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>2</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>50</v>
       </c>
-      <c r="M2" t="b">
+      <c r="N2" t="b">
+        <v>1</v>
+      </c>
+      <c r="O2" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <dataValidations count="10">
+  <dataValidations count="12">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" prompt="The amount of experimental variables. This can be either 2 (Condition A, Replicates) or 3 (Condition B, Condition A, Replicates). These variables should be present in the .raw file names._x000a_Condition A example: Cell lines_x000a_Condition B example: WT/KO" sqref="B2" xr:uid="{5282C8AD-1561-44E0-A80B-84CE01E96738}">
       <formula1>"2, 3"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" prompt="The type of comparison that will be tested. This can be all possible pairwise comparisons (&quot;all&quot;) or limited to the comparisons versus the control (&quot;control&quot;)." sqref="E2" xr:uid="{C495E0AF-0FD2-459F-A3CE-5F10744ED4BB}">
-      <formula1>"control, all"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Control sample" prompt="In case you choose &quot;control&quot; as your comparison, add the name of the control sample, e.g. DMSO, IgG, untreated, KO" sqref="F2" xr:uid="{FBBE24AB-7FB5-4AFC-8068-8D0236696CFE}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Control sample" prompt="In case you choose &quot;control&quot; as your comparison, add the name of the control sample, e.g. DMSO, IgG, untreated, KO" sqref="G2" xr:uid="{FBBE24AB-7FB5-4AFC-8068-8D0236696CFE}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Mass spectrometer" prompt="This should be present in the names of the .raw files. Required when selecting DiaNN as analysis method" sqref="D2" xr:uid="{68E78BE4-A7EB-420A-9A7C-D7D367FCB586}"/>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" prompt="This indicates the type of filtering_x000a__x000a_- complete: valid values in all samples_x000a_- condition: valid values in all samples of at least one group/condition" sqref="C2" xr:uid="{9FC734E1-D13B-4158-8BC3-0C7F48EE5CBD}">
       <formula1>"complete, condition"</formula1>
@@ -556,14 +575,21 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{01EF4A6D-0D3B-42B5-ADF2-F19004687B57}">
       <formula1>"DiaNN, MaxQuant, Proteome Discoverer"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The minimum amount of unique peptides a protein should be quantified with" sqref="G2" xr:uid="{A31E311C-361E-4F9F-B8B6-BC4E0E89553B}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Specifiy which proteins to highlight in the volcano plot._x000a_- list of supplied protein names_x000a_- all proteins above a supplied p-value and fold change cutoff_x000a_- the top N most differential proteins with a p-value &lt; 0.05" sqref="H2" xr:uid="{A788C50D-30A4-4BCA-985C-C9490DA02A01}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The minimum amount of unique peptides a protein should be quantified with" sqref="H2" xr:uid="{A31E311C-361E-4F9F-B8B6-BC4E0E89553B}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Specifiy which proteins to highlight in the volcano plot._x000a_- list of supplied protein names_x000a_- all proteins above a supplied p-value and fold change cutoff_x000a_- the top N most differential proteins with a p-value &lt; 0.05" sqref="I2" xr:uid="{A788C50D-30A4-4BCA-985C-C9490DA02A01}">
       <formula1>"protein list, specify significance, TopN"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="List of proteins, separated by a semiolon (;)" sqref="I2" xr:uid="{E5F7B0FE-6278-49BC-987F-F5F080EF479D}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2" xr:uid="{BFA4E188-76D8-454E-913F-287D42E85D9F}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="List of proteins, separated by a semiolon (;)" sqref="J2" xr:uid="{E5F7B0FE-6278-49BC-987F-F5F080EF479D}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:O2" xr:uid="{BFA4E188-76D8-454E-913F-287D42E85D9F}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N1" xr:uid="{05F39213-E70C-4B6E-8638-D660A08C4561}">
+      <formula1>"TRUE, FALSE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" prompt="The type of comparison that will be tested. This can be all possible pairwise comparisons (&quot;all&quot;), a manual selection (&quot;manual&quot;) or limited to the comparisons versus the control (&quot;control&quot;)." sqref="E2" xr:uid="{CAE86A27-1E22-4258-9B9C-34B30B1C0743}">
+      <formula1>"control, manual, all"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Contrasts" prompt="In case you choose &quot;manual&quot; as your comparison, add the comparisons you would like to make, separated by a semicolon. E.g. C1_vs_DMSO;DMSO_vs_IgG" sqref="F2" xr:uid="{2B445CE9-19EB-4F5A-AB70-882C1276BC70}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>